<commit_message>
added more time for antispam timeout
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -19,28 +19,61 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>First Date</t>
+    <t>Question</t>
   </si>
   <si>
-    <t>Question</t>
+    <t>Вопрос 11: Интересно, что, когда в 1891 году ПЕРВЫЙ сломал ногу во время экспедиции, его сумел вылечить ВТОРОЙ. Назовите обоих.
+Ответ: [Роберт] Пири, [Фредерик] Кук.
+Комментарий: Фредерик Кук был врачом гренландской экспедиции Пири. Впоследствии они стали врагами, споря за приоритет в открытии Северного полюса.</t>
+  </si>
+  <si>
+    <t>Вопрос 6: В описании официального ИКСА России упоминаются Михаил Барклай-де-Толли и еще один Михаил. Назовите ИКС.
+Ответ: Тартан.
+Зачёт: Килт.
+Комментарий: Официальный тартан России состоит из тартанов Барклая и Лермонтова, которые были выходцами из Шотландии.</t>
+  </si>
+  <si>
+    <t>Вопрос 15 Святослав Рихтер утверждал, что ВТОРОЕ способно произвести гораздо больший эффект, чем ПЕРВОЕ. Назовите ПЕРВОЕ и ВТОРОЕ.
+Ответ: Форте, пиано.
+Зачёт: По корням слов (например, "фортиссимо, пианиссимо").
+Комментарий: Рихтер говорил о концертном исполнении фортепианных произведений, но можно отнести его замечание и к более широкому контексту: громко не значит эффективно.</t>
+  </si>
+  <si>
+    <t>Вопрос 34: Согласно фанатской теории, основой для которой стали два события прошлого десятилетия, ОНА является метафорой эстроге́на. Назовите ЕЁ двумя словами, которые НЕ начинаются на соседние буквы алфавита.
+Ответ: красная таблетка.
+Комментарий: красная таблетка позволила Нео увидеть реальность такой, какая она есть на самом деле. Согласно фанатской теории, красная таблетка является прямой отсылкой к эстрогену — гормону, принимаемому при смене пола. В интервью 2020 года Лилли Вачовски заявила, что фильм «Матрица» подчёркивает проблемы трансгендерной идентичности.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -51,7 +84,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -59,11 +92,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -81,10 +129,16 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -366,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -382,283 +436,320 @@
     <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C1" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="146.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="3">
-        <f>E27</f>
-        <v>45471</v>
-      </c>
-      <c r="C2" s="6"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="7">
+        <v>45485</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="159.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="3">
-        <f>B2</f>
-        <v>45471</v>
-      </c>
-      <c r="C3" s="6"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="7">
+        <v>45485</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="199.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="3">
-        <f>B3</f>
-        <v>45471</v>
-      </c>
-      <c r="C4" s="6"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="7">
+        <v>45485</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="252" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="3">
-        <f>B4+1</f>
-        <v>45472</v>
-      </c>
-      <c r="C5" s="6"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="7">
+        <v>45485</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="3">
-        <f>B5</f>
-        <v>45472</v>
-      </c>
-      <c r="C6" s="6"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="7"/>
+      <c r="C6" s="9"/>
+    </row>
+    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="3">
-        <f>B6</f>
-        <v>45472</v>
-      </c>
-      <c r="C7" s="6"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+    </row>
+    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="3">
-        <f>B7+1</f>
-        <v>45473</v>
-      </c>
-      <c r="C8" s="6"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+    </row>
+    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="3">
-        <f>B8</f>
-        <v>45473</v>
-      </c>
-      <c r="C9" s="6"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+    </row>
+    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="3">
-        <f>B9</f>
-        <v>45473</v>
-      </c>
-      <c r="C10" s="6"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+    </row>
+    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="3">
-        <f>B10+1</f>
-        <v>45474</v>
-      </c>
-      <c r="C11" s="6"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+    </row>
+    <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="3">
-        <f>B11</f>
-        <v>45474</v>
-      </c>
-      <c r="C12" s="6"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+    </row>
+    <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="3">
-        <f>B12</f>
-        <v>45474</v>
-      </c>
-      <c r="C13" s="6"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+    </row>
+    <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="3">
-        <f>B13+1</f>
-        <v>45475</v>
-      </c>
-      <c r="C14" s="6"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+    </row>
+    <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="3">
-        <f>B14</f>
-        <v>45475</v>
-      </c>
-      <c r="C15" s="6"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+    </row>
+    <row r="16" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="3">
-        <f>B15</f>
-        <v>45475</v>
-      </c>
-      <c r="C16" s="6"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B16" s="7"/>
+      <c r="C16" s="9"/>
+    </row>
+    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="3">
-        <f>B16+1</f>
-        <v>45476</v>
-      </c>
-      <c r="C17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+    </row>
+    <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" s="3">
-        <f>B17</f>
-        <v>45476</v>
-      </c>
-      <c r="C18" s="6"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
+    </row>
+    <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="3">
-        <f>B18</f>
-        <v>45476</v>
-      </c>
-      <c r="C19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B19" s="7"/>
+      <c r="C19" s="8"/>
+    </row>
+    <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" s="3">
-        <f>B19+1</f>
-        <v>45477</v>
-      </c>
-      <c r="C20" s="6"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
+    </row>
+    <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" s="3">
-        <f>B20</f>
-        <v>45477</v>
-      </c>
-      <c r="C21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B21" s="7"/>
+      <c r="C21" s="9"/>
+    </row>
+    <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" s="3">
-        <f>B21</f>
-        <v>45477</v>
-      </c>
-      <c r="C22" s="6"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="3"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="3"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B25" s="3"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B26" s="3"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B27" s="3"/>
-      <c r="D27" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E27" s="4">
-        <v>45471</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B28" s="3"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B29" s="3"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B30" s="3"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B31" s="3"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B32" s="3"/>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B33" s="3"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B34" s="3"/>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B35" s="3"/>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B36" s="3"/>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B37" s="3"/>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B38" s="3"/>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B39" s="3"/>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B40" s="3"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="8"/>
+    </row>
+    <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="8"/>
+    </row>
+    <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" s="7"/>
+      <c r="C24" s="8"/>
+    </row>
+    <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="8"/>
+    </row>
+    <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="9"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" s="7"/>
+      <c r="C31" s="9"/>
+    </row>
+    <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" s="7"/>
+      <c r="C32" s="8"/>
+    </row>
+    <row r="33" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" s="7"/>
+      <c r="C33" s="8"/>
+    </row>
+    <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" s="7"/>
+      <c r="C34" s="8"/>
+    </row>
+    <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" s="7"/>
+      <c r="C35" s="8"/>
+    </row>
+    <row r="36" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="7"/>
+      <c r="C36" s="9"/>
+    </row>
+    <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="7"/>
+      <c r="C37" s="8"/>
+    </row>
+    <row r="38" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="7"/>
+      <c r="C38" s="8"/>
+    </row>
+    <row r="39" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="7"/>
+      <c r="C39" s="8"/>
+    </row>
+    <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="7"/>
+      <c r="C40" s="8"/>
+      <c r="E40" s="4"/>
+    </row>
+    <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="7"/>
+      <c r="C41" s="9"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B42" s="3"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B43" s="3"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B44" s="3"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B45" s="3"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B46" s="3"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B47" s="3"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B48" s="3"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49" s="3"/>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B50" s="3"/>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B51" s="3"/>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B52" s="3"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B53" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed post log output
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -19,12 +19,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Date</t>
   </si>
   <si>
     <t>Question</t>
+  </si>
+  <si>
+    <t>Вопрос 3:
+Раздаточный материал
+Homo sapiens — Culex pipiens — Homo sapiens — Haematopota pluvialis — Homo sapiens — Bombus proteus — Homo sapiens
+    По мнению автора вопроса, в результате этих метаморфоз пострадали три особы. Назовите всех троих.
+Ответ: Повариха, ткачиха, (сватья баба) Бабариха.
+Зачёт: В любом порядке.
+Комментарий: Данные метаморфозы претерпевал князь Гвидон. Culex pipiens [кУлекс пипиЕнс] — комар обыкновенный, Haematopota pluvialis [гематопОта плювиАлис] — слепень дождёвка обыкновенная (поскольку именно эта муха, обитающая в умеренной зоне, наносит наиболее болезненные укусы, автор вопроса посмел предположить, что именно она фигурирует в сказке Пушкина), Bombus proteus [бОмбус протЕус] — шмель обыкновенный.</t>
   </si>
   <si>
     <t>Вопрос 11: Интересно, что, когда в 1891 году ПЕРВЫЙ сломал ногу во время экспедиции, его сумел вылечить ВТОРОЙ. Назовите обоих.
@@ -111,7 +120,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -139,6 +148,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -422,8 +434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -452,7 +464,7 @@
         <v>45485</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="159.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -463,7 +475,7 @@
         <v>45485</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="199.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -474,7 +486,7 @@
         <v>45485</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="252" thickBot="1" x14ac:dyDescent="0.35">
@@ -485,15 +497,19 @@
         <v>45485</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="357.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="9"/>
+      <c r="B6" s="7">
+        <v>45485</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1">

</xml_diff>

<commit_message>
some fixes in readme
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -27,35 +27,35 @@
     <t>Question</t>
   </si>
   <si>
-    <t>Вопрос 3:
-Раздаточный материал
-Homo sapiens — Culex pipiens — Homo sapiens — Haematopota pluvialis — Homo sapiens — Bombus proteus — Homo sapiens
-    По мнению автора вопроса, в результате этих метаморфоз пострадали три особы. Назовите всех троих.
-Ответ: Повариха, ткачиха, (сватья баба) Бабариха.
-Зачёт: В любом порядке.
-Комментарий: Данные метаморфозы претерпевал князь Гвидон. Culex pipiens [кУлекс пипиЕнс] — комар обыкновенный, Haematopota pluvialis [гематопОта плювиАлис] — слепень дождёвка обыкновенная (поскольку именно эта муха, обитающая в умеренной зоне, наносит наиболее болезненные укусы, автор вопроса посмел предположить, что именно она фигурирует в сказке Пушкина), Bombus proteus [бОмбус протЕус] — шмель обыкновенный.</t>
+    <t>#N/A</t>
   </si>
   <si>
-    <t>Вопрос 11: Интересно, что, когда в 1891 году ПЕРВЫЙ сломал ногу во время экспедиции, его сумел вылечить ВТОРОЙ. Назовите обоих.
-Ответ: [Роберт] Пири, [Фредерик] Кук.
-Комментарий: Фредерик Кук был врачом гренландской экспедиции Пири. Впоследствии они стали врагами, споря за приоритет в открытии Северного полюса.</t>
+    <t>Вопрос 35: В древней легенде охотник спасся от преследования дикого зверя, воспользовавшись ИКСом. А затем даже смог убить зверя, попав тому в глаз, тем самым узнав одну из особенностей ИКСа. Кто написал «ИКС»?
+Ответ: Пушкин.
+Комментарий: охотник сначала залез на дерево, а потом опытным путем открыл, что это дерево содержит яды. ИКС – анчар. «Анчар» — известное стихотворение Пушкина, обличающее самодержавие.</t>
   </si>
   <si>
-    <t>Вопрос 6: В описании официального ИКСА России упоминаются Михаил Барклай-де-Толли и еще один Михаил. Назовите ИКС.
-Ответ: Тартан.
-Зачёт: Килт.
-Комментарий: Официальный тартан России состоит из тартанов Барклая и Лермонтова, которые были выходцами из Шотландии.</t>
+    <t>Вопрос 8: Назовите брахмана, написавшего песню "Ты, Господь душ всех людей".
+Ответ: Рабиндранат Тагор.
+Комментарий: Эта песня является национальным гимном Индии. Рабиндранат Тагор был выходцем из касты брахманов.</t>
   </si>
   <si>
-    <t>Вопрос 15 Святослав Рихтер утверждал, что ВТОРОЕ способно произвести гораздо больший эффект, чем ПЕРВОЕ. Назовите ПЕРВОЕ и ВТОРОЕ.
-Ответ: Форте, пиано.
-Зачёт: По корням слов (например, "фортиссимо, пианиссимо").
-Комментарий: Рихтер говорил о концертном исполнении фортепианных произведений, но можно отнести его замечание и к более широкому контексту: громко не значит эффективно.</t>
+    <t>Вопрос 7: Рассказывают, что в ЕГО рацион входило и грудное молоко, для чего при дворе приходилось содержать специальный штат кормилиц. В качестве примера "ЕГО" Википедия называет 105-этажную гостиницу "Рюгён" в Пхеньяне. Назовите ЕГО двумя словами.
+Ответ: Белый слон.
+Комментарий: Белый слон — священная реликвия нескольких королевских дворов Юго-Восточной Азии. По легенде, король Сиама предоставлял содержание своего белого слона неугодным придворным с целью их разорить. Идиома "белый слон" обозначает нечто дорогостоящее и бесполезное. Гостиница "Рюгён", спроектированная как самая высокая в мире, строится почти тридцать лет, хотя зачем такой отель в стране, где практически нет туристов, — не известно.</t>
   </si>
   <si>
-    <t>Вопрос 34: Согласно фанатской теории, основой для которой стали два события прошлого десятилетия, ОНА является метафорой эстроге́на. Назовите ЕЁ двумя словами, которые НЕ начинаются на соседние буквы алфавита.
-Ответ: красная таблетка.
-Комментарий: красная таблетка позволила Нео увидеть реальность такой, какая она есть на самом деле. Согласно фанатской теории, красная таблетка является прямой отсылкой к эстрогену — гормону, принимаемому при смене пола. В интервью 2020 года Лилли Вачовски заявила, что фильм «Матрица» подчёркивает проблемы трансгендерной идентичности.</t>
+    <t>Вопрос 18:
+https://iqga.me/upload/iblock/4c8/4c89257ed8bbb8b9c0a8c32b97a47e6f.png
+В родном городе известного голландца установили необычный фонтан. Конструкция cверху, выпускающая клубы пара, символизирует ЭТО. Назовите ЭТО двумя словами, начинающимися на одну и ту же букву.
+Ответ: облако Оорта
+Зачёт: точный ответ.
+Комментарий: памятник установили во Франекере – родном городе выдающегося астронома Яна Хендрика Оорта, автора идеи о существовании облака, из которого к нам приходят кометы. На снимке пар немного напоминает хвост кометы.</t>
+  </si>
+  <si>
+    <t>Вопрос 5: В статье, посвященной матчу между "Манчестер Юнайтед" и "Глазго Рейнджерс", говорится, что шотландцы бОльшую часть матча заботились об обороне. При этом команда сравнивалась с объектом, включенным в список Всемирного наследия. Назовите этот объект двумя словами.
+Ответ: Адрианов вал.
+Комментарий: Адрианов вал как раз проходит по территории Шотландии и построен для защиты.</t>
   </si>
 </sst>
 </file>
@@ -120,7 +120,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -131,9 +131,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -150,7 +147,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -432,340 +429,358 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="40" style="5" customWidth="1"/>
+    <col min="3" max="3" width="40" style="4" customWidth="1"/>
     <col min="4" max="4" width="19.88671875" style="1" customWidth="1"/>
     <col min="5" max="5" width="17.77734375" style="1" customWidth="1"/>
     <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="146.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="7">
-        <v>45485</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="159.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="9"/>
+    </row>
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="7">
-        <v>45485</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="199.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="9"/>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="7">
-        <v>45485</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="252" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="6"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="9"/>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="7">
-        <v>45485</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="357.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="9"/>
+    </row>
+    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="7">
-        <v>45485</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="6"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-    </row>
-    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-    </row>
-    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-    </row>
-    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-    </row>
-    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="6"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="7"/>
+      <c r="B11" s="6"/>
       <c r="C11" s="8"/>
-    </row>
-    <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-    </row>
-    <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-    </row>
-    <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="6"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-    </row>
-    <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="9"/>
+    </row>
+    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-    </row>
-    <row r="16" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="9"/>
+    </row>
+    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="9"/>
-    </row>
-    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="6"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-    </row>
-    <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="9"/>
+    </row>
+    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-    </row>
-    <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="9"/>
+    </row>
+    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
-    </row>
-    <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="9"/>
+    </row>
+    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-    </row>
-    <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="9"/>
+    </row>
+    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="9"/>
-    </row>
-    <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="6"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="8"/>
-    </row>
-    <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="6"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="9"/>
+    </row>
+    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="8"/>
-    </row>
-    <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="9"/>
+    </row>
+    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="8"/>
-    </row>
-    <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="6"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="9"/>
+    </row>
+    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="8"/>
-    </row>
-    <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="6"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="9"/>
+    </row>
+    <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="9"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B26" s="6"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+    </row>
+    <row r="27" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B27" s="6"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="9"/>
+    </row>
+    <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B28" s="6"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="9"/>
+    </row>
+    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="6"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="9"/>
+    </row>
+    <row r="30" spans="1:4" ht="199.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="6">
+        <v>45491</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="9"/>
+    </row>
+    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>29</v>
       </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="9"/>
-    </row>
-    <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="6">
+        <v>45491</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="8"/>
+    </row>
+    <row r="32" spans="1:4" ht="133.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="8"/>
-    </row>
-    <row r="33" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="6">
+        <v>45492</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="9"/>
+    </row>
+    <row r="33" spans="1:4" ht="291.60000000000002" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>31</v>
       </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="8"/>
-    </row>
-    <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="6">
+        <v>45492</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="9"/>
+    </row>
+    <row r="34" spans="1:4" ht="265.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>32</v>
       </c>
-      <c r="B34" s="7"/>
-      <c r="C34" s="8"/>
-    </row>
-    <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="6">
+        <v>45492</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="9"/>
+    </row>
+    <row r="35" spans="1:4" ht="186" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>33</v>
       </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="8"/>
-    </row>
-    <row r="36" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="7"/>
-      <c r="C36" s="9"/>
-    </row>
-    <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="7"/>
-      <c r="C37" s="8"/>
-    </row>
-    <row r="38" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="7"/>
-      <c r="C38" s="8"/>
-    </row>
-    <row r="39" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="7"/>
-      <c r="C39" s="8"/>
-    </row>
-    <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="7"/>
-      <c r="C40" s="8"/>
-      <c r="E40" s="4"/>
-    </row>
-    <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="7"/>
-      <c r="C41" s="9"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B35" s="6">
+        <v>45492</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="9"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B36" s="3"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B37" s="3"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B38" s="3"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B39" s="3"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B40" s="3"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B41" s="3"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B42" s="3"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B43" s="3"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B44" s="3"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B45" s="3"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B46" s="3"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B47" s="3"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B48" s="3"/>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B49" s="3"/>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B50" s="3"/>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B51" s="3"/>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B52" s="3"/>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B53" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
another try to fix antispam issue
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -30,32 +30,141 @@
     <t>#N/A</t>
   </si>
   <si>
-    <t>Вопрос 35: В древней легенде охотник спасся от преследования дикого зверя, воспользовавшись ИКСом. А затем даже смог убить зверя, попав тому в глаз, тем самым узнав одну из особенностей ИКСа. Кто написал «ИКС»?
-Ответ: Пушкин.
-Комментарий: охотник сначала залез на дерево, а потом опытным путем открыл, что это дерево содержит яды. ИКС – анчар. «Анчар» — известное стихотворение Пушкина, обличающее самодержавие.</t>
-  </si>
-  <si>
-    <t>Вопрос 8: Назовите брахмана, написавшего песню "Ты, Господь душ всех людей".
-Ответ: Рабиндранат Тагор.
-Комментарий: Эта песня является национальным гимном Индии. Рабиндранат Тагор был выходцем из касты брахманов.</t>
-  </si>
-  <si>
-    <t>Вопрос 7: Рассказывают, что в ЕГО рацион входило и грудное молоко, для чего при дворе приходилось содержать специальный штат кормилиц. В качестве примера "ЕГО" Википедия называет 105-этажную гостиницу "Рюгён" в Пхеньяне. Назовите ЕГО двумя словами.
-Ответ: Белый слон.
-Комментарий: Белый слон — священная реликвия нескольких королевских дворов Юго-Восточной Азии. По легенде, король Сиама предоставлял содержание своего белого слона неугодным придворным с целью их разорить. Идиома "белый слон" обозначает нечто дорогостоящее и бесполезное. Гостиница "Рюгён", спроектированная как самая высокая в мире, строится почти тридцать лет, хотя зачем такой отель в стране, где практически нет туристов, — не известно.</t>
-  </si>
-  <si>
-    <t>Вопрос 18:
-https://iqga.me/upload/iblock/4c8/4c89257ed8bbb8b9c0a8c32b97a47e6f.png
-В родном городе известного голландца установили необычный фонтан. Конструкция cверху, выпускающая клубы пара, символизирует ЭТО. Назовите ЭТО двумя словами, начинающимися на одну и ту же букву.
-Ответ: облако Оорта
-Зачёт: точный ответ.
-Комментарий: памятник установили во Франекере – родном городе выдающегося астронома Яна Хендрика Оорта, автора идеи о существовании облака, из которого к нам приходят кометы. На снимке пар немного напоминает хвост кометы.</t>
-  </si>
-  <si>
-    <t>Вопрос 5: В статье, посвященной матчу между "Манчестер Юнайтед" и "Глазго Рейнджерс", говорится, что шотландцы бОльшую часть матча заботились об обороне. При этом команда сравнивалась с объектом, включенным в список Всемирного наследия. Назовите этот объект двумя словами.
-Ответ: Адрианов вал.
-Комментарий: Адрианов вал как раз проходит по территории Шотландии и построен для защиты.</t>
+    <t>корабль дураков босха</t>
+  </si>
+  <si>
+    <t>Тео ван Гог</t>
+  </si>
+  <si>
+    <t>Бейлис, дело Бейлиса</t>
+  </si>
+  <si>
+    <t>HAL 9000</t>
+  </si>
+  <si>
+    <t>буба кики</t>
+  </si>
+  <si>
+    <t>десять дней кот. потрясли</t>
+  </si>
+  <si>
+    <t>Превращение» кафка</t>
+  </si>
+  <si>
+    <t>Кнут Гамсун Голод</t>
+  </si>
+  <si>
+    <t>Дэмьен Херст</t>
+  </si>
+  <si>
+    <t>Вопрос 6:
+https://db.chgk.info/images/db/20160803.jpg
+    Перед вами нижний фрагмент иллюстрации к научной статье. Если на нем распознаётся, пожалуй, самая известная АЛЬФА — значит, задача ИКСА решена качественно. АЛЬФА ИКСА — символ профессионального лицемерия. Что мы заменили АЛЬФОЙ ИКСА?
+Ответ: Улыбка коммивояжера.
+Комментарий: АЛЬФА — улыбка. ИКС — коммивояжер. Статья посвящена использованию критерия понятности получающихся изображений для оценки качества методов оптимальной маршрутизации (задачи коммивояжера). В данном случае исходное изображение — Мона Лиза.</t>
+  </si>
+  <si>
+    <t>Вопрос 9: В этом вопросе ИКС заменяет словосочетание.
+    Пароход "Грейт Истерн" был настолько огромен, что, по выражению шутников, пассажиры парохода могли бы иметь своего ИКСА. ИКСОВ сейчас 659, и их принято называть двумя буквами. Напишите эти буквы.
+Ответ: MP [чтецу: эм-пи].
+Комментарий: Пассажиров могло быть до четырех тысяч, что давало бы право избирать своего представителя в палате общин. По итогам последних на данный момент выборов в Палате общин 659 членов. Членов Парламента сокращают до MP — Members of Parliament.</t>
+  </si>
+  <si>
+    <t>Вопрос 32: Психолог Гелена Савицкая проводит аналогии между людьми и архитектурными элементами. С чем она сравнивает женщин, которые много на себя берут и пытаются всё контролировать, но реальной пользы почти не приносят?
+Ответ: С кариатидой.
+Комментарий: В реальном мире кариатида пользы приносит куда меньше, чем можно предположить по виду.</t>
+  </si>
+  <si>
+    <t>Вопрос 13: Этот глагол стоит под номером 42 в известном собрании середины XIX века. Этот же глагол, только на другом языке и во множественном числе, завершает произведение середины XX века. Назовите автора второго произведения.
+Ответ: [Юлиус] Фучик.
+Комментарий: Глагол — "Бди!" (К. Прутков, "Мысли и афоризмы", N 42), у Фучика — "Bděte!", что перевели на русский как "Будьте бдительны!".</t>
+  </si>
+  <si>
+    <t>Вопрос 14: Один человек рассказывает, что, обучаясь на факультете искусствоведения, писал дипломную работу по творчеству художника Ива Кляйна в том числе по некой причине. А на первом курсе преподаватель по той же причине посоветовал ему специализироваться на античной скульптуре. Назовите эту причину словом английского происхождения.
+Ответ: Дальтонизм.
+Зачёт: Дальтоник.
+Комментарий: Ив Кляйн известен своими монохромными работами. Для многих работ он использовал синий цвет, который был назван в его честь — так называемый "международный синий цвет Кляйна". Для того чтобы изучать античную скульптуру, различать цвета не обязательно. Актер Эдди Редмэйн, получивший искусствоведческое образование, — дальтоник.</t>
+  </si>
+  <si>
+    <t>Вопрос 13:
+https://db.chgk.info/images/db/20140087.jpg
+    Пешеходный маршрут, который проходит вдоль всего побережья Бретани, носит название "тропа ИКСОВ". Назовите ИКСА.
+Ответ: Таможенник.
+Комментарий: Бретань с ее неровным рельефом и большой протяженностью береговой линии была излюбленным местом нелегальной выгрузки товаров. Поэтому для борьбы с контрабандистами здесь была проложена так называемая "тропа таможенников", которая в наши дни стала туристическим маршрутом. Мы раздали вам посвященную Бретани картину художника-примитивиста Анри Руссо, который носил прозвище Таможенник.</t>
+  </si>
+  <si>
+    <t>Вопрос 11: Некоторые переводчики предпочли вставить между первыми двумя словами этого произведения междометие "о". Назовите это произведение.
+Ответ: "The Tyger".
+Зачёт: "Тигр"; "Тигр, тигр"; "Тигр, о тигр...".
+Комментарий: Интересно, что были еще и переводчики, колебавшиеся в выборе. В более позднем варианте перевода знаменитого стихотворения Уильяма Блейка Самуил Маршак вставил в стихотворение междометие "о", что не изменило размер стихотворения. Строки перевода звучат, соответственно, как "Тигр, тигр — огонь, горящий..." и "Тигр, о тигр, светло горящий".</t>
+  </si>
+  <si>
+    <t>Вопрос 9: В одном из фильмов Шерлок Холмс сравнивает своего брата и его клуб со всюду лезущей секретной службой. Стоит, мол, начаться волнениям в Судане, как рядом оказывается экспедиция, направленная клубом к истокам Нила, а беспорядки в Гималаях не обходятся без искателей снежного человека. В русской озвучке Холмс характеризует клуб поговоркой из четырех слов. Воспроизведите ее.
+Ответ: В каждой бочке затычка.
+Зачёт: К каждой бочке затычка.
+Комментарий: Поговорка используется для описания человека, который непрошено вмешивается во все дела. И по смыслу подходит, и названию клуба "Диоген" хорошо соответствует. В оригинале Холмс говорит, что "Диоген" is here, there, and everywhere.</t>
+  </si>
+  <si>
+    <t>Вопрос 24:   Внимание, в данном вопросе мы дважды пропустили одни и те же три буквы.
+    Известный человек однажды заявил, что "Сталин — гигант, а все западные деятели — геи". Считается, что в "галионе" этот человек отразил свое многолетнее увлечение фонетикой. Назовите этого человека.
+Ответ: [Джордж Бернард] Шоу.
+Комментарий: Мы дважды пропустили буквы "П", "И", "М" в буквосочетании -ПИГМ-. На самом деле Бернард Шоу называл западных деятелей пигмеями. Во второй части вопроса речь идет о его пьесе "Пигмалион".</t>
+  </si>
+  <si>
+    <t>Вопрос 14: В годы пребывания ТАМ английский мистик семнадцатого века Элино́р Дэ́вис считала себя Девой Марией в пещере. Ответьте точно: где ТАМ?
+Ответ: в Бедла́ме.
+Зачёт: по слову «Бедлам».
+Комментарий: английская лечебница для душевнобольных «Бедлам» получила своё название в честь города Вифлеем. Будучи обитательницей Бедлама, Дэвис называла себя Девой Марией, которая вот-вот родит Христа.</t>
+  </si>
+  <si>
+    <t>Вопрос 10: Из англоязычной фразы Эжена Ионеско трудно понять, какой маршрут он избрал для безумных пророков — из НАЗАРЕТА в ЛАЗАРЕТ или наоборот. Напишите на русском или английском языке в произвольном порядке слова, которые мы заменили словами "НАЗАРЕТ" и "ЛАЗАРЕТ".
+Ответ: Bethleham, Bethleham или Вифлеем, Бедлам.
+Зачёт: В любом порядке.
+Комментарий: Бедлам — больница для умалишенных в Лондоне, название которой произошло от названия города Вифлеем. Двусмысленная фраза Ионеско звучит как "from Bethleham to Bethleham".</t>
+  </si>
+  <si>
+    <t>Вопрос 7: В японской живописи эпохи Хэйан использовался прием “интерьера со снятой крышей”, создающий эффект ЕГО. “ОН” был опубликован в 1879 году. Назовите ЕГО двумя словами.
+Ответ: кукольный дом
+Зачёт: кукольный домик
+Комментарий: В японской живописи ямато-э периода Хэйан с VIII по XII век сцены в дворцовых покоях изображались сверху, как будто зритель заглядывал в кукольный домик и видел фрагмент помещения со скошен­ными балками, занавесями и сидящими в них героями. Пьеса Ибсена “Кукольный дом” была опубликована в 1879 году.</t>
+  </si>
+  <si>
+    <t>Вопрос 31:
+https://i.imgur.com/39vxMGp.png
+    По замечанию Анны Егоровой, рассматривая картины в стиле яма́то-э́, зритель будто бы заглядывает в НЕГО. Впервые «ОН» был представлен публике в 1879 году. Назовите ЕГО.
+Ответ: Кукольный дом.
+Зачёт: Кукольный домик.
+Комментарий: В ямато-э дворцы часто изображали со снятой крышей и стеной. В этом случае художник и зрители наблюдают дворцовые залы, словно заглядывая в кукольный домик. Пьеса Ге́нрика И́бсена «Кукольный дом» впервые была поставлена в 1879 в Королевском театре Копенгагена.</t>
+  </si>
+  <si>
+    <t>Вопрос 10: В вопросе есть замена.
+    Оливер Сакс в книге "Человек, который принял жену за шляпу" рассказывает о женщине, которая утратила идею "левой стороны", т.е. не видела ничего, что находилось слева, — например, еду на левой стороне тарелки. Она выработала стратегии, позволяющие обойти дефект: так, если ей казалось, что на тарелке не хватает еды, она начинала вертеться на кресле-каталке вправо. Доехав по кругу до недостающей половины, она съедала половину еды, и если всё еще была голодна, то делала еще один оборот, и т.д. Таким образом, пациентка Сакса сравнила себя с бочкой Диогена. Какие слова мы заменили в этом вопросе?
+Ответ: Стрела Зенона.
+Комментарий: "Абсурд, — говорит она. — Я как стрела Зенона — никогда не долетаю до цели. Выглядит это, наверно, как в цирке, но куда же денешься?".</t>
+  </si>
+  <si>
+    <t>Вопрос 11:   Математик Сергей Бобров удалил верхний левый фрагмент из того, что можно увидеть на "НЕЙ". В результате он получил позицию, для которой несложно найти решение. Идея другой "ЕЕ" зародилась во время сеанса психотерапии. Назовите ЕЕ.
+Ответ: Меланхолия.
+Зачёт: "Меланхолия".
+Комментарий: Бобров, который был не только математиком, но и художником, вытащил из магического квадрата, изображенного на "Меланхолии" Дюрера, верхний левый фрагмент с числом 16. Для получившейся позиции игры "15" несложно найти алгоритм, который позволяет переставить числа в порядке возрастания. Уроженцу Копенгагена Ларсу фон Триеру идея фильма "Меланхолия" пришла во время лечения от депрессии.</t>
+  </si>
+  <si>
+    <t>Вопрос 11:
+https://db.chgk.info/images/db/20120370.jpg
+    Перед вами фрагмент картины Дюрера "Четыре апостола". Крайний справа — Павел. По распространенному мнению, на картине Павел олицетворяет, в частности, ЭТО. ЭТО во времена Дюрера считалось присущим гениям. Назовите ЭТО.
+Ответ: Меланхолия.
+Комментарий: Четыре апостола представляют четыре разных типа темперамента. У Дюрера есть известнейшая гравюра "Меланхолия".</t>
+  </si>
+  <si>
+    <t>Вопрос 6: Джон Мэн пишет, что в шестнадцатом веке ОН объявлял об интересных новинках и служил хорошей рекламой. Назовите ЕГО.
+Ответ: Индекс запрещенных книг.
+Зачёт: Список запрещенных книг.
+Комментарий: Благодаря включению новой книги в список запрещенных книг о ней узнавали потенциальные издатели и читатели.</t>
+  </si>
+  <si>
+    <t>Вопрос 66: Когда с книгой Фердинанда Грегоровиуса "История Рима в Средние века" произошло это, его поздравляли с высокой честью. Автор лично отправился проверить это в Собор святого Петра. Что же случилось с книгой?
+Ответ: Она попала в "Индекс запрещенных книг".
+Комментарий: Грегоровиус не был большим любителем католической церкви. В Соборе святого Петра вывешивались списки новых книг, попавших в Индекс.</t>
   </si>
 </sst>
 </file>
@@ -120,19 +229,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -146,8 +246,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -429,134 +529,437 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="40" style="4" customWidth="1"/>
+    <col min="3" max="3" width="40" style="2" customWidth="1"/>
     <col min="4" max="4" width="19.88671875" style="1" customWidth="1"/>
     <col min="5" max="5" width="17.77734375" style="1" customWidth="1"/>
     <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="186" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
+        <v>45516</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="6"/>
+    </row>
+    <row r="3" spans="1:4" ht="199.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <v>45516</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="252" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <v>45516</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="186" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <v>45516</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <v>45516</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3">
+        <v>45517</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="304.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3">
+        <v>45517</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="252" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3">
+        <v>45517</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3">
+        <v>45517</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3">
+        <v>45517</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3">
+        <v>45518</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="172.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3">
+        <v>45518</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="6">
-        <v>45491</v>
-      </c>
-      <c r="C2" s="7" t="s">
+    </row>
+    <row r="14" spans="1:4" ht="265.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3">
+        <v>45518</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" s="3">
+        <v>45518</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="3">
+        <v>45518</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" s="3">
+        <v>45519</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="9"/>
-    </row>
-    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
+    </row>
+    <row r="18" spans="1:3" ht="331.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="3">
+        <v>45519</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="318" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="3">
+        <v>45519</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="3">
+        <v>45519</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" s="3">
+        <v>45519</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" s="3">
+        <v>45520</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="199.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" s="3">
+        <v>45520</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="304.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" s="3">
+        <v>45520</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="172.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" s="3">
+        <v>45520</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" s="3">
+        <v>45520</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" s="3">
+        <v>45521</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" s="3">
+        <v>45521</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="186" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" s="3">
+        <v>45521</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="6">
-        <v>45491</v>
-      </c>
-      <c r="C3" s="8" t="s">
+    </row>
+    <row r="30" spans="1:3" ht="252" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" s="3">
+        <v>45521</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="3">
+        <v>45521</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="8"/>
-    </row>
-    <row r="4" spans="1:4" ht="106.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
-        <v>30</v>
-      </c>
-      <c r="B4" s="6">
-        <v>45492</v>
-      </c>
-      <c r="C4" s="7" t="s">
+    </row>
+    <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="3">
+        <v>45522</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="3">
+        <v>45522</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" ht="265.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="3">
+        <v>45522</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" ht="278.39999999999998" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="3">
+        <v>45522</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="3">
+        <v>45522</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="3">
+        <v>45523</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="3">
+        <v>45523</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="1:4" ht="291.60000000000002" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
-        <v>31</v>
-      </c>
-      <c r="B5" s="6">
-        <v>45492</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="9"/>
-    </row>
-    <row r="6" spans="1:4" ht="265.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
-        <v>32</v>
-      </c>
-      <c r="B6" s="6">
-        <v>45492</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="1:4" ht="186" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
-        <v>33</v>
-      </c>
-      <c r="B7" s="6">
-        <v>45492</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="3"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="3"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="3"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B14" s="3"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B15" s="3"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" s="3"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B18" s="3"/>
+    </row>
+    <row r="39" spans="2:3" ht="238.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="3">
+        <v>45523</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" ht="238.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="3">
+        <v>45523</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="3">
+        <v>45523</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>